<commit_message>
hw6 pt 2 big upload
</commit_message>
<xml_diff>
--- a/geog370hw6pt1/bachelorsdegreedata.xlsx
+++ b/geog370hw6pt1/bachelorsdegreedata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hornacob/Desktop/dev/Geog370/geog370hw3/geog370hw6pt1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9C40096B-1BD1-154B-B3E7-85206D8997F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B4CD5-62CA-F340-987E-F29B28D09566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="7800" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACSST5Y2020.S1501-Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t>GEO_ID</t>
   </si>
@@ -648,12 +648,15 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>Sum- overall total population</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1490,17 +1493,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -1519,7 +1523,9 @@
       <c r="E1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1547,7 +1553,10 @@
         <f>C2+D2</f>
         <v>29383</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2">
+        <f>SUM(D2,E2)</f>
+        <v>57684</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1575,7 +1584,10 @@
         <f t="shared" ref="E3:E66" si="0">C3+D3</f>
         <v>4060</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">SUM(D3,E3)</f>
+        <v>7886</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1603,7 +1615,10 @@
         <f t="shared" si="0"/>
         <v>1887</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>3655</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1631,7 +1646,10 @@
         <f t="shared" si="0"/>
         <v>2089</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4041</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1659,7 +1677,10 @@
         <f t="shared" si="0"/>
         <v>4285</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8409</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1687,7 +1708,10 @@
         <f t="shared" si="0"/>
         <v>3238</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6409</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1715,7 +1739,10 @@
         <f t="shared" si="0"/>
         <v>7273</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>14386</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1743,7 +1770,10 @@
         <f t="shared" si="0"/>
         <v>2094</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4168</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1771,7 +1801,10 @@
         <f t="shared" si="0"/>
         <v>4400</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>8744</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1799,7 +1832,10 @@
         <f t="shared" si="0"/>
         <v>32484</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>64617</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1827,7 +1863,10 @@
         <f t="shared" si="0"/>
         <v>81249</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>160571</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1855,7 +1894,10 @@
         <f t="shared" si="0"/>
         <v>11486</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>22523</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1883,7 +1925,10 @@
         <f t="shared" si="0"/>
         <v>48993</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>96116</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1911,7 +1956,10 @@
         <f t="shared" si="0"/>
         <v>9847</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>19216</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1939,7 +1987,10 @@
         <f t="shared" si="0"/>
         <v>1559</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>3083</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1967,7 +2018,10 @@
         <f t="shared" si="0"/>
         <v>15338</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>30374</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1995,7 +2049,10 @@
         <f t="shared" si="0"/>
         <v>2844</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>5453</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2023,7 +2080,10 @@
         <f t="shared" si="0"/>
         <v>26740</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>52127</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2051,7 +2111,10 @@
         <f t="shared" si="0"/>
         <v>23993</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>47509</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2079,7 +2142,10 @@
         <f t="shared" si="0"/>
         <v>4936</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>9741</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2107,7 +2173,10 @@
         <f t="shared" si="0"/>
         <v>2351</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>4658</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2135,7 +2204,10 @@
         <f t="shared" si="0"/>
         <v>2347</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>4694</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2163,7 +2235,10 @@
         <f t="shared" si="0"/>
         <v>13736</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>26871</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2191,7 +2266,10 @@
         <f t="shared" si="0"/>
         <v>5302</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>10370</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2219,7 +2297,10 @@
         <f t="shared" si="0"/>
         <v>17510</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>34409</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2247,7 +2328,10 @@
         <f t="shared" si="0"/>
         <v>55890</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>109073</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2275,7 +2359,10 @@
         <f t="shared" si="0"/>
         <v>5076</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>9989</v>
+      </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -2303,7 +2390,10 @@
         <f t="shared" si="0"/>
         <v>10901</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>21459</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2331,7 +2421,10 @@
         <f t="shared" si="0"/>
         <v>23592</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>45818</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2359,7 +2452,10 @@
         <f t="shared" si="0"/>
         <v>7569</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>14966</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2387,7 +2483,10 @@
         <f t="shared" si="0"/>
         <v>6056</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>11894</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2415,7 +2514,10 @@
         <f t="shared" si="0"/>
         <v>115300</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>223753</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2443,7 +2545,10 @@
         <f t="shared" si="0"/>
         <v>6075</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>11954</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2471,7 +2576,10 @@
         <f t="shared" si="0"/>
         <v>90634</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>176975</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2499,7 +2607,10 @@
         <f t="shared" si="0"/>
         <v>10404</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>20450</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2527,7 +2638,10 @@
         <f t="shared" si="0"/>
         <v>35234</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>69215</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2555,7 +2669,10 @@
         <f t="shared" si="0"/>
         <v>1109</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>2154</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2583,7 +2700,10 @@
         <f t="shared" si="0"/>
         <v>819</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>1638</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2611,7 +2731,10 @@
         <f t="shared" si="0"/>
         <v>10396</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>20499</v>
+      </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2639,7 +2762,10 @@
         <f t="shared" si="0"/>
         <v>1594</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>3155</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2667,7 +2793,10 @@
         <f t="shared" si="0"/>
         <v>136050</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>266416</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2695,7 +2824,10 @@
         <f t="shared" si="0"/>
         <v>5401</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>10692</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2723,7 +2855,10 @@
         <f t="shared" si="0"/>
         <v>20270</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>39612</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -2751,7 +2886,10 @@
         <f t="shared" si="0"/>
         <v>13485</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>26455</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2779,7 +2917,10 @@
         <f t="shared" si="0"/>
         <v>27900</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>55252</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2807,7 +2948,10 @@
         <f t="shared" si="0"/>
         <v>2808</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>5462</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -2835,7 +2979,10 @@
         <f t="shared" si="0"/>
         <v>6621</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>13093</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2863,7 +3010,10 @@
         <f t="shared" si="0"/>
         <v>402</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>804</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -2891,7 +3041,10 @@
         <f t="shared" si="0"/>
         <v>37873</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>74571</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2919,7 +3072,10 @@
         <f t="shared" si="0"/>
         <v>8630</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>16598</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -2947,7 +3103,10 @@
         <f t="shared" si="0"/>
         <v>33096</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>65580</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -2975,7 +3134,10 @@
         <f t="shared" si="0"/>
         <v>1068</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>2085</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -3003,7 +3165,10 @@
         <f t="shared" si="0"/>
         <v>8806</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>17289</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -3031,7 +3196,10 @@
         <f t="shared" si="0"/>
         <v>6446</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>12543</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -3059,7 +3227,10 @@
         <f t="shared" si="0"/>
         <v>14592</v>
       </c>
-      <c r="F56" s="1"/>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>28628</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -3087,7 +3258,10 @@
         <f t="shared" si="0"/>
         <v>6348</v>
       </c>
-      <c r="F57" s="1"/>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>12457</v>
+      </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -3115,7 +3289,10 @@
         <f t="shared" si="0"/>
         <v>6491</v>
       </c>
-      <c r="F58" s="1"/>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>12840</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3143,7 +3320,10 @@
         <f t="shared" si="0"/>
         <v>4851</v>
       </c>
-      <c r="F59" s="1"/>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>9545</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -3171,7 +3351,10 @@
         <f t="shared" si="0"/>
         <v>2587</v>
       </c>
-      <c r="F60" s="1"/>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>5069</v>
+      </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -3199,7 +3382,10 @@
         <f t="shared" si="0"/>
         <v>355427</v>
       </c>
-      <c r="F61" s="1"/>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>694017</v>
+      </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -3227,7 +3413,10 @@
         <f t="shared" si="0"/>
         <v>2529</v>
       </c>
-      <c r="F62" s="1"/>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>4993</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3255,7 +3444,10 @@
         <f t="shared" si="0"/>
         <v>3293</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>6401</v>
+      </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -3283,7 +3475,10 @@
         <f t="shared" si="0"/>
         <v>28380</v>
       </c>
-      <c r="F64" s="1"/>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>56251</v>
+      </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -3311,7 +3506,10 @@
         <f t="shared" si="0"/>
         <v>14495</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>28337</v>
+      </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -3339,7 +3537,10 @@
         <f t="shared" si="0"/>
         <v>70835</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>138065</v>
+      </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -3364,10 +3565,13 @@
         <v>2263</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E101" si="1">C67+D67</f>
+        <f t="shared" ref="E67:E101" si="2">C67+D67</f>
         <v>2263</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67">
+        <f t="shared" ref="F67:F101" si="3">SUM(D67,E67)</f>
+        <v>4526</v>
+      </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -3392,10 +3596,13 @@
         <v>25116</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26385</v>
       </c>
-      <c r="F68" s="1"/>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>51501</v>
+      </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -3420,10 +3627,13 @@
         <v>55545</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59900</v>
       </c>
-      <c r="F69" s="1"/>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>115445</v>
+      </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -3448,10 +3658,13 @@
         <v>2152</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2188</v>
       </c>
-      <c r="F70" s="1"/>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>4340</v>
+      </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -3476,10 +3689,13 @@
         <v>6342</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6545</v>
       </c>
-      <c r="F71" s="1"/>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>12887</v>
+      </c>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -3504,10 +3720,13 @@
         <v>12616</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12778</v>
       </c>
-      <c r="F72" s="1"/>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>25394</v>
+      </c>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -3532,10 +3751,13 @@
         <v>1992</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2007</v>
       </c>
-      <c r="F73" s="1"/>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>3999</v>
+      </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
@@ -3560,10 +3782,13 @@
         <v>4444</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4596</v>
       </c>
-      <c r="F74" s="1"/>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>9040</v>
+      </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -3588,10 +3813,13 @@
         <v>35349</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39063</v>
       </c>
-      <c r="F75" s="1"/>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>74412</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
@@ -3616,10 +3844,13 @@
         <v>5265</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5372</v>
       </c>
-      <c r="F76" s="1"/>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>10637</v>
+      </c>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -3644,10 +3875,13 @@
         <v>16071</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16597</v>
       </c>
-      <c r="F77" s="1"/>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>32668</v>
+      </c>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -3672,10 +3906,13 @@
         <v>5443</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5618</v>
       </c>
-      <c r="F78" s="1"/>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>11061</v>
+      </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -3700,10 +3937,13 @@
         <v>11970</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12396</v>
       </c>
-      <c r="F79" s="1"/>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>24366</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -3728,10 +3968,13 @@
         <v>10019</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10246</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>20265</v>
+      </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -3756,10 +3999,13 @@
         <v>19334</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20144</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>39478</v>
+      </c>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -3784,10 +4030,13 @@
         <v>9247</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9717</v>
       </c>
-      <c r="F82" s="1"/>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>18964</v>
+      </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -3812,10 +4061,13 @@
         <v>6132</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6482</v>
       </c>
-      <c r="F83" s="1"/>
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>12614</v>
+      </c>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
@@ -3840,10 +4092,13 @@
         <v>3665</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3876</v>
       </c>
-      <c r="F84" s="1"/>
+      <c r="F84">
+        <f t="shared" si="3"/>
+        <v>7541</v>
+      </c>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -3868,10 +4123,13 @@
         <v>7679</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8004</v>
       </c>
-      <c r="F85" s="1"/>
+      <c r="F85">
+        <f t="shared" si="3"/>
+        <v>15683</v>
+      </c>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -3896,10 +4154,13 @@
         <v>4503</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4616</v>
       </c>
-      <c r="F86" s="1"/>
+      <c r="F86">
+        <f t="shared" si="3"/>
+        <v>9119</v>
+      </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -3924,10 +4185,13 @@
         <v>9103</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9560</v>
       </c>
-      <c r="F87" s="1"/>
+      <c r="F87">
+        <f t="shared" si="3"/>
+        <v>18663</v>
+      </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -3952,10 +4216,13 @@
         <v>2018</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2047</v>
       </c>
-      <c r="F88" s="1"/>
+      <c r="F88">
+        <f t="shared" si="3"/>
+        <v>4065</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -3980,10 +4247,13 @@
         <v>8811</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8898</v>
       </c>
-      <c r="F89" s="1"/>
+      <c r="F89">
+        <f t="shared" si="3"/>
+        <v>17709</v>
+      </c>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -4008,10 +4278,13 @@
         <v>322</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>419</v>
       </c>
-      <c r="F90" s="1"/>
+      <c r="F90">
+        <f t="shared" si="3"/>
+        <v>741</v>
+      </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -4036,10 +4309,13 @@
         <v>54397</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56363</v>
       </c>
-      <c r="F91" s="1"/>
+      <c r="F91">
+        <f t="shared" si="3"/>
+        <v>110760</v>
+      </c>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -4064,10 +4340,13 @@
         <v>5288</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5448</v>
       </c>
-      <c r="F92" s="1"/>
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>10736</v>
+      </c>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -4092,8 +4371,12 @@
         <v>395000</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>416772</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="3"/>
+        <v>811772</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
@@ -4110,8 +4393,12 @@
         <v>2224</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2288</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="3"/>
+        <v>4512</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
@@ -4128,8 +4415,12 @@
         <v>1058</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1068</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>2126</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
@@ -4146,11 +4437,15 @@
         <v>13965</v>
       </c>
       <c r="E96" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15565</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <f t="shared" si="3"/>
+        <v>29530</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>194</v>
       </c>
@@ -4164,11 +4459,15 @@
         <v>16330</v>
       </c>
       <c r="E97" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16837</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <f t="shared" si="3"/>
+        <v>33167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>196</v>
       </c>
@@ -4182,11 +4481,15 @@
         <v>7888</v>
       </c>
       <c r="E98" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8117</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <f t="shared" si="3"/>
+        <v>16005</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>198</v>
       </c>
@@ -4200,11 +4503,15 @@
         <v>11154</v>
       </c>
       <c r="E99" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11774</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <f t="shared" si="3"/>
+        <v>22928</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>200</v>
       </c>
@@ -4218,11 +4525,15 @@
         <v>3475</v>
       </c>
       <c r="E100" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3694</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <f t="shared" si="3"/>
+        <v>7169</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>202</v>
       </c>
@@ -4236,8 +4547,12 @@
         <v>2706</v>
       </c>
       <c r="E101" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2748</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="3"/>
+        <v>5454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>